<commit_message>
Update STALKER Anomaly 1.5.1 - Mods Load Order.xlsx
- Add new Mods Load Order for 13th January 2022 (2 versions)
</commit_message>
<xml_diff>
--- a/Mods Load Order/STALKER Anomaly 1.5.1 - Mods Load Order.xlsx
+++ b/Mods Load Order/STALKER Anomaly 1.5.1 - Mods Load Order.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Desktop\STALKER-Anomaly---My-Mods-Collection\Mods Load Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3BC253-1E4C-4EF9-A57C-89745C84013F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1067CCA6-F9BE-4CBB-A652-CB2E32F78A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="15585" firstSheet="1" activeTab="2" xr2:uid="{9B3995F9-12C5-4747-9014-E3FA0CC0DF07}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="15585" firstSheet="4" activeTab="4" xr2:uid="{9B3995F9-12C5-4747-9014-E3FA0CC0DF07}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
     <sheet name="10th January 2022" sheetId="1" r:id="rId2"/>
     <sheet name="11th January 2022" sheetId="3" r:id="rId3"/>
+    <sheet name="13th January 2022-v1" sheetId="4" r:id="rId4"/>
+    <sheet name="13th January 2022-v2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="122">
   <si>
     <t>STALKER Anomaly 1.5.1</t>
   </si>
@@ -363,6 +365,45 @@
   </si>
   <si>
     <t>QOL - Decreased AI Hearing Distance (Bushes)</t>
+  </si>
+  <si>
+    <t>13th January 2022</t>
+  </si>
+  <si>
+    <t>QOL - Weapon Sway 0.5</t>
+  </si>
+  <si>
+    <t>QOL - Quest Items Droppable RC 18</t>
+  </si>
+  <si>
+    <t>QOL - Reworked Oufit Attachments 1.3</t>
+  </si>
+  <si>
+    <t>QOL - Suppressor Reworked 75 - Standard Anomaly 1.05.6</t>
+  </si>
+  <si>
+    <t>QOL - 01 Dynamic_NPC_Armor_Visuals NPCs_loot_outfits</t>
+  </si>
+  <si>
+    <t>Mod "Load Order" version 1</t>
+  </si>
+  <si>
+    <t>Mod "Load Order" version 2</t>
+  </si>
+  <si>
+    <t>QOL - Suppressor Reworked 50 - Standard Anomaly 1.05.6</t>
+  </si>
+  <si>
+    <t>QOL - NicerFlashlights Addon Taclight 1.6</t>
+  </si>
+  <si>
+    <t>QOL - Highlight New Items</t>
+  </si>
+  <si>
+    <t>QOL - Food Drugs Drinks Visual Accuracy Item Counts</t>
+  </si>
+  <si>
+    <t>QOL - NVR EFT Style Version Old DX10-9-8</t>
   </si>
 </sst>
 </file>
@@ -907,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD353995-0ADD-4861-8866-13013B5620DB}">
   <dimension ref="A1:A106"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection sqref="A1:A106"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFE2E16-5004-47B0-906D-4F440065C326}">
   <dimension ref="A1:A108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107:A108"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection sqref="A1:A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,4 +2038,1154 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB539C3-AD53-4345-BDDB-2FAFF6CECCC5}">
+  <dimension ref="A1:A111"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9EC281-FAAA-4EB7-AFDB-ECA92B170E37}">
+  <dimension ref="A1:A115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>